<commit_message>
Updated excel spreadsheet to newer format compatable with openpyxl
</commit_message>
<xml_diff>
--- a/Cost_of_Vehicle_Format_Master.xlsx
+++ b/Cost_of_Vehicle_Format_Master.xlsx
@@ -9,17 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="3255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>AMOUNT</t>
   </si>
@@ -78,6 +80,12 @@
     <t xml:space="preserve">PURCHASE PRICE + INTERNET FEE + BUYER FEE+ GATE FEE </t>
   </si>
   <si>
+    <t xml:space="preserve">KIND OF DAMAGE: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">INFORMATION:  </t>
+  </si>
+  <si>
     <t>SUBTOTAL OF LABORS</t>
   </si>
   <si>
@@ -93,7 +101,7 @@
     <t>KIND OF DAMAGE:</t>
   </si>
   <si>
-    <t>TYPE OF VEHICLE:</t>
+    <t xml:space="preserve">TYPE OF VEHICLE: </t>
   </si>
 </sst>
 </file>
@@ -104,7 +112,7 @@
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -139,13 +147,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -176,6 +177,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="8" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -183,7 +185,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -502,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:C49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -514,17 +515,21 @@
     <col min="2" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
         <v>0</v>
@@ -533,37 +538,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="9"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="10"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B9" s="4">
         <f>SUM(B5:B7)</f>
@@ -571,35 +570,35 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="9"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="10"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="4"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -637,8 +636,8 @@
       <c r="C25" s="4"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="8" t="s">
-        <v>21</v>
+      <c r="A26" s="9" t="s">
+        <v>23</v>
       </c>
       <c r="B26" s="4">
         <f>SUM(B12:B25)</f>
@@ -673,16 +672,16 @@
       <c r="B30" s="4">
         <v>0</v>
       </c>
-      <c r="C30" s="5"/>
+      <c r="C30" s="6"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="5"/>
+      <c r="C31" s="6"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B32" s="4">
         <f>SUM(B28:B30)</f>
@@ -691,7 +690,7 @@
       <c r="C32" s="4"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B33" s="9"/>
+      <c r="B33" s="10"/>
       <c r="C33" s="4"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -778,27 +777,27 @@
       <c r="B43" s="4">
         <v>0</v>
       </c>
-      <c r="C43" s="6"/>
+      <c r="C43" s="7"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="4"/>
-      <c r="C44" s="6"/>
+      <c r="C44" s="7"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B45" s="9">
+      <c r="A45" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" s="10">
         <f>SUM(B35:B43)</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B46" s="9"/>
+      <c r="B46" s="10"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B47" s="4">
@@ -808,23 +807,368 @@
       <c r="C47" s="4"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="7"/>
+      <c r="A48" s="8"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="7"/>
+      <c r="A49" s="8"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="44.28515625" customWidth="1"/>
+    <col min="2" max="3" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="4">
+        <v>5934</v>
+      </c>
+      <c r="C5" s="4">
+        <f>SUM(B5)</f>
+        <v>5934</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="4">
+        <v>40</v>
+      </c>
+      <c r="C7" s="4">
+        <f>SUM(B7)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="4"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="4"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="5"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="5"/>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="5"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22" s="5"/>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" s="5"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25" s="5"/>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B26" s="5"/>
+      <c r="C26" s="4">
+        <f>SUM(B10:B25)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B27" s="5"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B28" s="5"/>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B29" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B30" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B31" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B32" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="5">
+        <v>0</v>
+      </c>
+      <c r="C33" s="4"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="5">
+        <v>0</v>
+      </c>
+      <c r="C34" s="4"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="5">
+        <v>0</v>
+      </c>
+      <c r="C35" s="4"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="5">
+        <v>0</v>
+      </c>
+      <c r="C36" s="6"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="4">
+        <f>SUM(B29:B36)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C39" s="4"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="4">
+        <v>0</v>
+      </c>
+      <c r="C43" s="4"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="4">
+        <v>0</v>
+      </c>
+      <c r="C44" s="4"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" s="4">
+        <v>0</v>
+      </c>
+      <c r="C45" s="4"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" s="4">
+        <v>0</v>
+      </c>
+      <c r="C46" s="4"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" s="4">
+        <v>0</v>
+      </c>
+      <c r="C47" s="4"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" s="4">
+        <v>0</v>
+      </c>
+      <c r="C48" s="4"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="4">
+        <v>0</v>
+      </c>
+      <c r="C49" s="7">
+        <f>SUM(B41:B49)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="4"/>
+      <c r="C52" s="4">
+        <f>SUM(C5:C49)</f>
+        <v>5974</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="8"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="8"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>